<commit_message>
change the title  Task.xlsx to the  C4B Team Professional..xlsx
</commit_message>
<xml_diff>
--- a/C4B Team Professional..xlsx
+++ b/C4B Team Professional..xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>add  your picture and  name to the team section  .</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -312,6 +315,38 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -330,38 +365,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -370,6 +373,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -377,15 +389,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -405,12 +408,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="name" dataDxfId="0"/>
+    <tableColumn id="1" name="name" dataDxfId="2"/>
     <tableColumn id="2" name="Task" dataDxfId="1"/>
-    <tableColumn id="3" name="End the task" dataDxfId="2"/>
+    <tableColumn id="3" name="End the task" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -459,7 +462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,7 +497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,7 +709,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +747,9 @@
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">

</xml_diff>